<commit_message>
finished getting models for all the logs
</commit_message>
<xml_diff>
--- a/assignment3/discovery/fitnesses.xlsx
+++ b/assignment3/discovery/fitnesses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="52">
   <si>
     <t>Trace Fitness</t>
   </si>
@@ -103,6 +103,75 @@
   </si>
   <si>
     <t>0% nosie</t>
+  </si>
+  <si>
+    <t>0.9709066867264007</t>
+  </si>
+  <si>
+    <t>0.9666172677208206</t>
+  </si>
+  <si>
+    <t>0.31751824817518237</t>
+  </si>
+  <si>
+    <t>V_After</t>
+  </si>
+  <si>
+    <t>0.9482449014748755</t>
+  </si>
+  <si>
+    <t>0.930329856932684</t>
+  </si>
+  <si>
+    <t>0.31266149870801024</t>
+  </si>
+  <si>
+    <t>D_After</t>
+  </si>
+  <si>
+    <t>15 evetns</t>
+  </si>
+  <si>
+    <t>10% noise</t>
+  </si>
+  <si>
+    <t>0.8482961020461021</t>
+  </si>
+  <si>
+    <t>0.8490897528397525</t>
+  </si>
+  <si>
+    <t>0.9992424242424245</t>
+  </si>
+  <si>
+    <t>113.65</t>
+  </si>
+  <si>
+    <t>H_After</t>
+  </si>
+  <si>
+    <t>20% noise</t>
+  </si>
+  <si>
+    <t>18 events</t>
+  </si>
+  <si>
+    <t>K_After</t>
+  </si>
+  <si>
+    <t>17 events</t>
+  </si>
+  <si>
+    <t>0.9335383081844235</t>
+  </si>
+  <si>
+    <t>0.9103502558048012</t>
+  </si>
+  <si>
+    <t>0.32085561497326176</t>
+  </si>
+  <si>
+    <t>10%noise</t>
   </si>
 </sst>
 </file>
@@ -448,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>2</v>
       </c>
@@ -802,7 +871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>3</v>
       </c>
@@ -813,7 +882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>4</v>
       </c>
@@ -824,7 +893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>5</v>
       </c>
@@ -835,7 +904,7 @@
         <v>7385869565217390</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>6</v>
       </c>
@@ -846,7 +915,7 @@
         <v>1.76358695652173E+16</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>7</v>
       </c>
@@ -857,7 +926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>8</v>
       </c>
@@ -865,6 +934,414 @@
         <v>12</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="2">
+        <v>4782323600973230</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="2">
+        <v>9941581508515810</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>8</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2.44599483204134E+16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="2">
+        <v>4134108527131780</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>8</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
+        <v>3</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="1">
+        <v>4</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1.11666666666666E+16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="1">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1.81666666666666E+16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <v>8</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="1">
+        <v>2</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="1">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="1">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1.00802139037433E+16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
+        <v>6</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="2">
+        <v>2.04866310160427E+16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="1">
+        <v>8</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>